<commit_message>
Added missing info for sprint 1 and LOC
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iklein\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Stories" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -346,6 +351,15 @@
   </si>
   <si>
     <t>https://github.com/Maestrodobis/Calculator_546</t>
+  </si>
+  <si>
+    <t>what we are doing.  Pretty consitent</t>
+  </si>
+  <si>
+    <t>Making dumb mistakes.  Always error check when you go and there will be less bugs.</t>
+  </si>
+  <si>
+    <t>iklein@stevens.edu</t>
   </si>
 </sst>
 </file>
@@ -801,7 +815,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="139">
+  <cellStyleXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -941,8 +955,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1103,8 +1118,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="139" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="139">
+  <cellStyles count="140">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1243,10 +1259,19 @@
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1271,10 +1296,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0505807488894849"/>
-          <c:y val="0.0277777676517324"/>
+          <c:x val="5.0580748889484897E-2"/>
+          <c:y val="2.7777767651732399E-2"/>
           <c:w val="0.906899571343596"/>
-          <c:h val="0.822469443544239"/>
+          <c:h val="0.82246944354423901"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1290,10 +1315,10 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>41187.0</c:v>
+                  <c:v>41187</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41193.0</c:v>
+                  <c:v>41193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1305,10 +1330,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1325,11 +1350,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2092886104"/>
-        <c:axId val="2092889112"/>
+        <c:axId val="-1383870768"/>
+        <c:axId val="-1383871856"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2092886104"/>
+        <c:axId val="-1383870768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,14 +1364,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092889112"/>
+        <c:crossAx val="-1383871856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2092889112"/>
+        <c:axId val="-1383871856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1357,7 +1382,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092886104"/>
+        <c:crossAx val="-1383870768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1368,7 +1393,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1731,19 +1756,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="6.42578125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="10" customWidth="1"/>
-    <col min="4" max="5" width="20.5703125" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="10.7109375" style="10"/>
+    <col min="1" max="2" width="6.375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="8.625" style="10" customWidth="1"/>
+    <col min="4" max="5" width="20.625" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="10.75" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
         <v>13</v>
       </c>
@@ -1760,14 +1785,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>34</v>
       </c>
@@ -1777,12 +1802,14 @@
       <c r="C3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="70" t="s">
+        <v>101</v>
+      </c>
       <c r="E3" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>37</v>
       </c>
@@ -1799,7 +1826,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13" customHeight="1">
+    <row r="9" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="60" t="s">
         <v>27</v>
       </c>
@@ -1817,6 +1844,9 @@
     <mergeCell ref="A9:C9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1835,16 +1865,16 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.75" customWidth="1"/>
+    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="4" max="4" width="6.75" customWidth="1"/>
+    <col min="5" max="5" width="7.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>22</v>
       </c>
@@ -1861,14 +1891,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="16"/>
     </row>
-    <row r="3" spans="1:5" ht="14" thickBot="1">
+    <row r="3" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
         <v>61</v>
       </c>
@@ -1896,21 +1926,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.75" style="1"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1930,7 +1960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>41187</v>
       </c>
@@ -1950,7 +1980,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
         <v>41193</v>
       </c>
@@ -1962,14 +1992,14 @@
         <v>3</v>
       </c>
       <c r="D3" s="19">
-        <v>250</v>
+        <v>111</v>
       </c>
       <c r="E3" s="19">
         <v>120</v>
       </c>
       <c r="F3" s="20">
         <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
+        <v>55.5</v>
       </c>
     </row>
   </sheetData>
@@ -1990,24 +2020,24 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="10"/>
-    <col min="5" max="5" width="6.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="17"/>
-    <col min="10" max="16384" width="10.7109375" style="10"/>
+    <col min="1" max="1" width="7.75" style="10" customWidth="1"/>
+    <col min="2" max="2" width="24.625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="6.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="10.75" style="10"/>
+    <col min="5" max="5" width="6.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="7.375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="6.75" style="10" customWidth="1"/>
+    <col min="8" max="8" width="7.75" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.75" style="17"/>
+    <col min="10" max="16384" width="10.75" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="44" t="s">
         <v>3</v>
       </c>
@@ -2036,7 +2066,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="49" t="s">
         <v>42</v>
       </c>
@@ -2050,22 +2080,22 @@
         <v>21</v>
       </c>
       <c r="E2" s="11">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="F2" s="11">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="G2" s="11">
         <v>120</v>
       </c>
       <c r="H2" s="11">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="I2" s="50">
         <v>41188</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="51" t="s">
         <v>65</v>
       </c>
@@ -2082,7 +2112,7 @@
       <c r="H3" s="11"/>
       <c r="I3" s="50"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="51" t="s">
         <v>66</v>
       </c>
@@ -2099,7 +2129,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="50"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="51" t="s">
         <v>67</v>
       </c>
@@ -2116,7 +2146,7 @@
       <c r="H5" s="11"/>
       <c r="I5" s="50"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="67"/>
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
@@ -2127,7 +2157,7 @@
       <c r="H6" s="68"/>
       <c r="I6" s="69"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="49" t="s">
         <v>43</v>
       </c>
@@ -2141,22 +2171,22 @@
         <v>21</v>
       </c>
       <c r="E7" s="11">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="F7" s="11">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="G7" s="11">
         <v>120</v>
       </c>
       <c r="H7" s="11">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="I7" s="50">
         <v>41191</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="51" t="s">
         <v>68</v>
       </c>
@@ -2173,7 +2203,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="50"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="51" t="s">
         <v>69</v>
       </c>
@@ -2190,7 +2220,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="50"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="51" t="s">
         <v>70</v>
       </c>
@@ -2207,7 +2237,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="50"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="64"/>
       <c r="B11" s="65"/>
       <c r="C11" s="65"/>
@@ -2218,7 +2248,7 @@
       <c r="H11" s="65"/>
       <c r="I11" s="66"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="49" t="s">
         <v>44</v>
       </c>
@@ -2232,22 +2262,22 @@
         <v>21</v>
       </c>
       <c r="E12" s="11">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="F12" s="11">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="G12" s="11">
-        <v>120</v>
+        <v>19</v>
       </c>
       <c r="H12" s="11">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="I12" s="50">
         <v>41193</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="51" t="s">
         <v>31</v>
       </c>
@@ -2264,7 +2294,7 @@
       <c r="H13" s="11"/>
       <c r="I13" s="50"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="51" t="s">
         <v>32</v>
       </c>
@@ -2281,7 +2311,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="50"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="51" t="s">
         <v>33</v>
       </c>
@@ -2298,7 +2328,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="50"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="51" t="s">
         <v>80</v>
       </c>
@@ -2315,7 +2345,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="50"/>
     </row>
-    <row r="17" spans="1:9" ht="14" thickBot="1">
+    <row r="17" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="54" t="s">
         <v>81</v>
       </c>
@@ -2332,36 +2362,40 @@
       <c r="H17" s="52"/>
       <c r="I17" s="53"/>
     </row>
-    <row r="18" spans="1:9" ht="14" thickBot="1"/>
-    <row r="19" spans="1:9" ht="13" customHeight="1">
+    <row r="18" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="13" customHeight="1" thickBot="1">
+    <row r="20" spans="1:9" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B21" s="33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="B22" s="34"/>
-    </row>
-    <row r="23" spans="1:9" ht="14" thickBot="1">
+    <row r="22" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B22" s="34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="35"/>
     </row>
-    <row r="24" spans="1:9" ht="14" thickBot="1">
+    <row r="24" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="32"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B25" s="36" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14" thickBot="1">
-      <c r="B26" s="37"/>
+    <row r="26" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="37" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2387,21 +2421,21 @@
       <selection activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="10"/>
-    <col min="5" max="5" width="6.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="17"/>
-    <col min="10" max="16384" width="10.7109375" style="10"/>
+    <col min="1" max="1" width="7.75" style="10" customWidth="1"/>
+    <col min="2" max="2" width="24.625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="6.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="10.75" style="10"/>
+    <col min="5" max="5" width="6.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="7.375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="6.75" style="10" customWidth="1"/>
+    <col min="8" max="8" width="7.75" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.75" style="17"/>
+    <col min="10" max="16384" width="10.75" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -2430,35 +2464,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14" thickBot="1"/>
-    <row r="3" spans="1:9">
+    <row r="2" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14" thickBot="1">
+    <row r="4" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="38"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="34"/>
     </row>
-    <row r="7" spans="1:9" ht="14" thickBot="1">
+    <row r="7" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="35"/>
     </row>
-    <row r="8" spans="1:9" ht="14" thickBot="1">
+    <row r="8" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="32"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="36" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14" thickBot="1">
+    <row r="10" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="37"/>
     </row>
   </sheetData>
@@ -2481,21 +2515,21 @@
       <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="10"/>
-    <col min="5" max="5" width="6.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="17"/>
-    <col min="10" max="16384" width="10.7109375" style="10"/>
+    <col min="1" max="1" width="7.75" style="10" customWidth="1"/>
+    <col min="2" max="2" width="24.625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="6.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="10.75" style="10"/>
+    <col min="5" max="5" width="6.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="7.375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="6.75" style="10" customWidth="1"/>
+    <col min="8" max="8" width="7.75" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.75" style="17"/>
+    <col min="10" max="16384" width="10.75" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -2524,35 +2558,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14" thickBot="1"/>
-    <row r="3" spans="1:9">
+    <row r="2" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14" thickBot="1">
+    <row r="4" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="38"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="34"/>
     </row>
-    <row r="7" spans="1:9" ht="14" thickBot="1">
+    <row r="7" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="35"/>
     </row>
-    <row r="8" spans="1:9" ht="14" thickBot="1">
+    <row r="8" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="32"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="36" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14" thickBot="1">
+    <row r="10" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="37"/>
     </row>
   </sheetData>
@@ -2574,21 +2608,21 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="10"/>
-    <col min="5" max="5" width="6.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="10" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="17"/>
-    <col min="10" max="16384" width="10.7109375" style="10"/>
+    <col min="1" max="1" width="7.75" style="10" customWidth="1"/>
+    <col min="2" max="2" width="24.625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="6.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="10.75" style="10"/>
+    <col min="5" max="5" width="6.875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="7.375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="6.75" style="10" customWidth="1"/>
+    <col min="8" max="8" width="7.75" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.75" style="17"/>
+    <col min="10" max="16384" width="10.75" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -2617,35 +2651,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14" thickBot="1"/>
-    <row r="3" spans="1:9">
+    <row r="2" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14" thickBot="1">
+    <row r="4" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="38"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" s="33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="34"/>
     </row>
-    <row r="7" spans="1:9" ht="14" thickBot="1">
+    <row r="7" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="35"/>
     </row>
-    <row r="8" spans="1:9" ht="14" thickBot="1">
+    <row r="8" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="32"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="36" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14" thickBot="1">
+    <row r="10" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="37"/>
     </row>
   </sheetData>
@@ -2667,15 +2701,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="10"/>
-    <col min="2" max="2" width="24.5703125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" style="21" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="10"/>
+    <col min="1" max="1" width="10.75" style="10"/>
+    <col min="2" max="2" width="24.625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="49.375" style="21" customWidth="1"/>
+    <col min="4" max="16384" width="10.75" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="15">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
@@ -2686,7 +2720,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1">
+    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="57" t="s">
         <v>42</v>
       </c>
@@ -2697,7 +2731,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" customHeight="1">
+    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="57" t="s">
         <v>43</v>
       </c>
@@ -2708,7 +2742,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1">
+    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="57" t="s">
         <v>44</v>
       </c>
@@ -2719,7 +2753,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1">
+    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="57" t="s">
         <v>45</v>
       </c>
@@ -2730,7 +2764,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="57" t="s">
         <v>46</v>
       </c>
@@ -2741,7 +2775,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="57" t="s">
         <v>47</v>
       </c>
@@ -2752,7 +2786,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="57" t="s">
         <v>48</v>
       </c>
@@ -2763,7 +2797,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="57" t="s">
         <v>49</v>
       </c>
@@ -2774,7 +2808,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" customHeight="1">
+    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="57" t="s">
         <v>50</v>
       </c>
@@ -2785,7 +2819,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" customHeight="1">
+    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="57" t="s">
         <v>51</v>
       </c>
@@ -2796,7 +2830,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31" thickBot="1">
+    <row r="12" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
         <v>91</v>
       </c>
@@ -2807,100 +2841,100 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C15" s="10"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="3:3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="3:3">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C18" s="10"/>
     </row>
-    <row r="19" spans="3:3">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="3:3">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C20" s="10"/>
     </row>
-    <row r="21" spans="3:3">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="3:3">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C22" s="10"/>
     </row>
-    <row r="23" spans="3:3">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C23" s="10"/>
     </row>
-    <row r="24" spans="3:3">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C24" s="10"/>
     </row>
-    <row r="25" spans="3:3">
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C25" s="10"/>
     </row>
-    <row r="26" spans="3:3">
+    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C26" s="10"/>
     </row>
-    <row r="27" spans="3:3">
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C27" s="10"/>
     </row>
-    <row r="28" spans="3:3">
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C28" s="10"/>
     </row>
-    <row r="29" spans="3:3">
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C29" s="10"/>
     </row>
-    <row r="30" spans="3:3">
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C30" s="10"/>
     </row>
-    <row r="31" spans="3:3">
+    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C31" s="10"/>
     </row>
-    <row r="32" spans="3:3">
+    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C32" s="10"/>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" s="10"/>
     </row>
-    <row r="34" spans="3:3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" s="10"/>
     </row>
-    <row r="35" spans="3:3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C35" s="10"/>
     </row>
-    <row r="36" spans="3:3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C36" s="10"/>
     </row>
-    <row r="37" spans="3:3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C37" s="10"/>
     </row>
-    <row r="38" spans="3:3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C38" s="10"/>
     </row>
-    <row r="39" spans="3:3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C39" s="10"/>
     </row>
-    <row r="40" spans="3:3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C40" s="10"/>
     </row>
-    <row r="41" spans="3:3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C41" s="10"/>
     </row>
-    <row r="42" spans="3:3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C42" s="10"/>
     </row>
-    <row r="43" spans="3:3">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C43" s="10"/>
     </row>
-    <row r="44" spans="3:3">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C44" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprint 3 log updated.
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iklein\Documents\cs555\Calculator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" tabRatio="500" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Stories" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="149">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -221,6 +216,9 @@
     <t>Catch error if a number is divided by zero and display alert box saying "Division by ZERO not possible!"</t>
   </si>
   <si>
+    <t>Develop 'division(/)' button that performs substraction operation on the input.</t>
+  </si>
+  <si>
     <t>Develop 'Reset' button that resets the entire calculator.</t>
   </si>
   <si>
@@ -356,9 +354,15 @@
     <t>Addition Operation</t>
   </si>
   <si>
+    <t>Develop '+' button that performs multiplication operation on the input.</t>
+  </si>
+  <si>
     <t>Substraction Operation</t>
   </si>
   <si>
+    <t>Develop '-' button that performs multiplication operation on the input.</t>
+  </si>
+  <si>
     <t>Multiplication Operation</t>
   </si>
   <si>
@@ -440,13 +444,58 @@
     <t xml:space="preserve">          Develop '/' button with same dimensions</t>
   </si>
   <si>
-    <t>Develop '-' button that performs subtraction operation on the input.</t>
-  </si>
-  <si>
-    <t>Develop '+' button that performs addition operation on the input.</t>
-  </si>
-  <si>
-    <t>Develop 'division(/)' button that performs division operation on the input.</t>
+    <t>JC13</t>
+  </si>
+  <si>
+    <t>Display Numbers on Screen</t>
+  </si>
+  <si>
+    <t>Develop a logic that displays the types numbers.</t>
+  </si>
+  <si>
+    <t>T07.01</t>
+  </si>
+  <si>
+    <t>T07.02</t>
+  </si>
+  <si>
+    <t>T07.03</t>
+  </si>
+  <si>
+    <t>T08.01</t>
+  </si>
+  <si>
+    <t>T08.02</t>
+  </si>
+  <si>
+    <t>T08.03</t>
+  </si>
+  <si>
+    <t>Display numbers on screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Set dimensions for reset button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Position the button appropriately</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Reset and Clear the screen on-click</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Set font of the printed numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Set the alignment of the numbers printed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Display numbers on the screen</t>
+  </si>
+  <si>
+    <t>Finish before deadline.</t>
+  </si>
+  <si>
+    <t>Keep the code structure clean and maintain indentation.</t>
   </si>
 </sst>
 </file>
@@ -762,7 +811,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="146">
+  <cellStyleXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -909,8 +958,52 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1077,8 +1170,23 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="146">
+  <cellStyles count="190">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1170,6 +1278,28 @@
     <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1224,6 +1354,28 @@
     <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1260,10 +1412,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.0580748889484897E-2"/>
-          <c:y val="2.7777767651732399E-2"/>
+          <c:x val="0.0505807488894849"/>
+          <c:y val="0.0277777676517324"/>
           <c:w val="0.906899571343596"/>
-          <c:h val="0.82246944354423901"/>
+          <c:h val="0.822469443544239"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1279,13 +1431,16 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>41187</c:v>
+                  <c:v>41187.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41193</c:v>
+                  <c:v>41193.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41200</c:v>
+                  <c:v>41200.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41221.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1297,13 +1452,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1320,11 +1478,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1070633648"/>
-        <c:axId val="-1070629296"/>
+        <c:axId val="2087116520"/>
+        <c:axId val="2088079224"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1070633648"/>
+        <c:axId val="2087116520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1334,14 +1492,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1070629296"/>
+        <c:crossAx val="2088079224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1070629296"/>
+        <c:axId val="2088079224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1352,7 +1510,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1070633648"/>
+        <c:crossAx val="2087116520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1363,7 +1521,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1730,15 +1888,15 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="6.375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.625" style="7" customWidth="1"/>
-    <col min="4" max="5" width="20.625" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="10.75" style="7"/>
+    <col min="1" max="2" width="6.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="7" customWidth="1"/>
+    <col min="4" max="5" width="20.5703125" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="10.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="19" t="s">
         <v>13</v>
       </c>
@@ -1755,14 +1913,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="9" t="s">
         <v>34</v>
       </c>
@@ -1773,13 +1931,13 @@
         <v>36</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
         <v>37</v>
       </c>
@@ -1796,14 +1954,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="13" customHeight="1">
       <c r="A9" s="58" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="58"/>
       <c r="C9" s="58"/>
       <c r="D9" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1826,22 +1984,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="7.75" customWidth="1"/>
-    <col min="3" max="3" width="19.375" customWidth="1"/>
-    <col min="4" max="4" width="6.75" customWidth="1"/>
-    <col min="5" max="5" width="7.75" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="35" t="s">
         <v>22</v>
       </c>
@@ -1858,7 +2016,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="40">
         <v>2</v>
       </c>
@@ -1866,16 +2024,16 @@
         <v>45</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E2" s="52" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="40">
         <v>2</v>
       </c>
@@ -1883,44 +2041,27 @@
         <v>46</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="40">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="61"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14" thickBot="1">
+      <c r="A4" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A4:E4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1935,23 +2076,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" style="1"/>
-    <col min="2" max="2" width="16.75" customWidth="1"/>
-    <col min="3" max="3" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1962,41 +2103,41 @@
         <v>2</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="12">
         <v>41187</v>
       </c>
       <c r="B2" s="13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D2" s="13">
         <v>0</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="12">
         <v>41193</v>
       </c>
       <c r="B3" s="13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="13">
         <f>B2-B3</f>
@@ -2013,12 +2154,12 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="12">
         <v>41200</v>
       </c>
       <c r="B4" s="13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="13">
         <f>B3-B4</f>
@@ -2033,6 +2174,28 @@
       <c r="F4" s="14">
         <f>(D4-D3)/E4*60</f>
         <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="12">
+        <v>41221</v>
+      </c>
+      <c r="B5" s="13">
+        <v>5</v>
+      </c>
+      <c r="C5" s="13">
+        <f>B4-B5</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="13">
+        <v>290</v>
+      </c>
+      <c r="E5" s="13">
+        <v>160</v>
+      </c>
+      <c r="F5" s="14">
+        <f>(D5-D4)/E5*60</f>
+        <v>40.875</v>
       </c>
     </row>
   </sheetData>
@@ -2052,25 +2215,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="150" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="7" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="15" customWidth="1"/>
-    <col min="3" max="3" width="6.75" style="7" customWidth="1"/>
-    <col min="4" max="4" width="10.75" style="7"/>
-    <col min="5" max="5" width="6.875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="7.375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="6.75" style="7" customWidth="1"/>
-    <col min="8" max="8" width="7.75" style="7" customWidth="1"/>
-    <col min="9" max="9" width="10.75" style="11"/>
-    <col min="10" max="16384" width="10.75" style="7"/>
+    <col min="1" max="1" width="7.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="7"/>
+    <col min="5" max="5" width="6.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="11"/>
+    <col min="10" max="16384" width="10.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -2099,12 +2262,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="40" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>34</v>
@@ -2128,12 +2291,12 @@
         <v>41188</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="42" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>34</v>
@@ -2145,12 +2308,12 @@
       <c r="H3" s="8"/>
       <c r="I3" s="41"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="42" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>34</v>
@@ -2162,12 +2325,12 @@
       <c r="H4" s="8"/>
       <c r="I4" s="41"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="42" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C5" s="33" t="s">
         <v>34</v>
@@ -2179,7 +2342,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="41"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="65"/>
       <c r="B6" s="66"/>
       <c r="C6" s="66"/>
@@ -2190,12 +2353,12 @@
       <c r="H6" s="66"/>
       <c r="I6" s="67"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="40" t="s">
         <v>43</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>34</v>
@@ -2219,12 +2382,12 @@
         <v>41191</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="42" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C8" s="33" t="s">
         <v>34</v>
@@ -2236,12 +2399,12 @@
       <c r="H8" s="8"/>
       <c r="I8" s="41"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="42" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>34</v>
@@ -2253,12 +2416,12 @@
       <c r="H9" s="8"/>
       <c r="I9" s="41"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C10" s="33" t="s">
         <v>34</v>
@@ -2270,7 +2433,7 @@
       <c r="H10" s="8"/>
       <c r="I10" s="41"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="62"/>
       <c r="B11" s="63"/>
       <c r="C11" s="63"/>
@@ -2281,12 +2444,12 @@
       <c r="H11" s="63"/>
       <c r="I11" s="64"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="40" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>34</v>
@@ -2310,12 +2473,12 @@
         <v>41193</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="42" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" s="33" t="s">
         <v>34</v>
@@ -2327,12 +2490,12 @@
       <c r="H13" s="8"/>
       <c r="I13" s="41"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="42" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C14" s="33" t="s">
         <v>34</v>
@@ -2344,12 +2507,12 @@
       <c r="H14" s="8"/>
       <c r="I14" s="41"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="42" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" s="33" t="s">
         <v>34</v>
@@ -2361,12 +2524,12 @@
       <c r="H15" s="8"/>
       <c r="I15" s="41"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C16" s="33" t="s">
         <v>34</v>
@@ -2378,12 +2541,12 @@
       <c r="H16" s="8"/>
       <c r="I16" s="41"/>
     </row>
-    <row r="17" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="14" thickBot="1">
       <c r="A17" s="45" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C17" s="47" t="s">
         <v>34</v>
@@ -2395,39 +2558,39 @@
       <c r="H17" s="43"/>
       <c r="I17" s="44"/>
     </row>
-    <row r="18" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="14" thickBot="1"/>
+    <row r="19" spans="1:9" ht="13" customHeight="1">
       <c r="B19" s="30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="13" customHeight="1" thickBot="1">
       <c r="B20" s="29"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="B21" s="24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="B22" s="25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14" thickBot="1">
       <c r="B23" s="26"/>
     </row>
-    <row r="24" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="14" thickBot="1">
       <c r="B24" s="23"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="B25" s="27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="40" thickBot="1">
       <c r="B26" s="28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2450,25 +2613,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A5" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="7" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="15" customWidth="1"/>
-    <col min="3" max="3" width="6.75" style="7" customWidth="1"/>
-    <col min="4" max="4" width="10.75" style="7"/>
-    <col min="5" max="5" width="6.875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="7.375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="6.75" style="7" customWidth="1"/>
-    <col min="8" max="8" width="7.75" style="7" customWidth="1"/>
-    <col min="9" max="9" width="10.75" style="11"/>
-    <col min="10" max="16384" width="10.75" style="7"/>
+    <col min="1" max="1" width="7.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="7"/>
+    <col min="5" max="5" width="6.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="11"/>
+    <col min="10" max="16384" width="10.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
@@ -2497,12 +2660,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="40" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>37</v>
@@ -2526,12 +2689,12 @@
         <v>41195</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="42" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>37</v>
@@ -2543,12 +2706,12 @@
       <c r="H3" s="8"/>
       <c r="I3" s="41"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="42" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>37</v>
@@ -2560,12 +2723,12 @@
       <c r="H4" s="8"/>
       <c r="I4" s="41"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="42" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C5" s="33" t="s">
         <v>37</v>
@@ -2577,7 +2740,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="41"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="65"/>
       <c r="B6" s="66"/>
       <c r="C6" s="66"/>
@@ -2588,12 +2751,12 @@
       <c r="H6" s="66"/>
       <c r="I6" s="67"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="40" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>34</v>
@@ -2617,12 +2780,12 @@
         <v>41198</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="42" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C8" s="33" t="s">
         <v>34</v>
@@ -2634,12 +2797,12 @@
       <c r="H8" s="8"/>
       <c r="I8" s="41"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9" s="42" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>34</v>
@@ -2651,12 +2814,12 @@
       <c r="H9" s="8"/>
       <c r="I9" s="41"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="42" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C10" s="33" t="s">
         <v>34</v>
@@ -2668,7 +2831,7 @@
       <c r="H10" s="8"/>
       <c r="I10" s="41"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="62"/>
       <c r="B11" s="63"/>
       <c r="C11" s="63"/>
@@ -2679,12 +2842,12 @@
       <c r="H11" s="63"/>
       <c r="I11" s="64"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="40" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>34</v>
@@ -2708,12 +2871,12 @@
         <v>41200</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="42" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C13" s="33" t="s">
         <v>34</v>
@@ -2725,12 +2888,12 @@
       <c r="H13" s="8"/>
       <c r="I13" s="41"/>
     </row>
-    <row r="14" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="42" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C14" s="33" t="s">
         <v>37</v>
@@ -2742,12 +2905,12 @@
       <c r="H14" s="8"/>
       <c r="I14" s="41"/>
     </row>
-    <row r="15" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="42" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C15" s="33" t="s">
         <v>37</v>
@@ -2759,12 +2922,12 @@
       <c r="H15" s="8"/>
       <c r="I15" s="41"/>
     </row>
-    <row r="16" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="42" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C16" s="33" t="s">
         <v>34</v>
@@ -2776,12 +2939,12 @@
       <c r="H16" s="8"/>
       <c r="I16" s="41"/>
     </row>
-    <row r="17" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="14" thickBot="1">
       <c r="A17" s="42" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B17" s="46" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C17" s="47" t="s">
         <v>34</v>
@@ -2793,39 +2956,39 @@
       <c r="H17" s="43"/>
       <c r="I17" s="44"/>
     </row>
-    <row r="18" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:9" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="14" thickBot="1"/>
+    <row r="19" spans="1:9" ht="13" customHeight="1">
       <c r="B19" s="30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="12.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="13" customHeight="1" thickBot="1">
       <c r="B20" s="29"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="B21" s="24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="26">
       <c r="B22" s="25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14" thickBot="1">
       <c r="B23" s="26"/>
     </row>
-    <row r="24" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="14" thickBot="1">
       <c r="B24" s="23"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="B25" s="27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="27" thickBot="1">
       <c r="B26" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2846,89 +3009,284 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="7" customWidth="1"/>
-    <col min="2" max="2" width="24.625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="6.75" style="7" customWidth="1"/>
-    <col min="4" max="4" width="10.75" style="7"/>
-    <col min="5" max="5" width="6.875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="7.375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="6.75" style="7" customWidth="1"/>
-    <col min="8" max="8" width="7.75" style="7" customWidth="1"/>
-    <col min="9" max="9" width="10.75" style="11"/>
-    <col min="10" max="16384" width="10.75" style="7"/>
+    <col min="1" max="1" width="7.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="7"/>
+    <col min="5" max="5" width="6.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="11"/>
+    <col min="10" max="16384" width="10.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="39" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="30" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="8">
+        <v>30</v>
+      </c>
+      <c r="F2" s="8">
+        <v>25</v>
+      </c>
+      <c r="G2" s="8">
+        <v>35</v>
+      </c>
+      <c r="H2" s="8">
+        <v>25</v>
+      </c>
+      <c r="I2" s="41">
+        <v>41210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="41"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="41"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="41"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="65"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="67"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="8">
+        <v>50</v>
+      </c>
+      <c r="F7" s="8">
+        <v>30</v>
+      </c>
+      <c r="G7" s="8">
+        <v>46</v>
+      </c>
+      <c r="H7" s="8">
+        <v>35</v>
+      </c>
+      <c r="I7" s="41">
+        <v>41216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="34"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="41"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="34"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="41"/>
+    </row>
+    <row r="10" spans="1:9" ht="14" thickBot="1">
+      <c r="A10" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="46" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="69"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="44"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="68"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+    </row>
+    <row r="12" spans="1:9" ht="14" thickBot="1"/>
+    <row r="13" spans="1:9">
+      <c r="B13" s="30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="29"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="24" t="s">
+    <row r="14" spans="1:9" ht="14" thickBot="1">
+      <c r="B14" s="29"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" s="24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="25"/>
-    </row>
-    <row r="7" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-    </row>
-    <row r="8" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="27" t="s">
+    <row r="16" spans="1:9">
+      <c r="B16" s="25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="14" thickBot="1">
+      <c r="B17" s="26"/>
+    </row>
+    <row r="18" spans="2:2" ht="14" thickBot="1">
+      <c r="B18" s="23"/>
+    </row>
+    <row r="19" spans="2:2" ht="13" customHeight="1">
+      <c r="B19" s="27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
+    <row r="20" spans="2:2" ht="13" customHeight="1">
+      <c r="B20" s="71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="14" thickBot="1">
+      <c r="B21" s="72"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="B20:B21"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2945,21 +3303,21 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.75" style="7" customWidth="1"/>
-    <col min="2" max="2" width="24.625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="6.75" style="7" customWidth="1"/>
-    <col min="4" max="4" width="10.75" style="7"/>
-    <col min="5" max="5" width="6.875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="7.375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="6.75" style="7" customWidth="1"/>
-    <col min="8" max="8" width="7.75" style="7" customWidth="1"/>
-    <col min="9" max="9" width="10.75" style="11"/>
-    <col min="10" max="16384" width="10.75" style="7"/>
+    <col min="1" max="1" width="7.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="7"/>
+    <col min="5" max="5" width="6.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="11"/>
+    <col min="10" max="16384" width="10.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
@@ -2988,35 +3346,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="14" thickBot="1"/>
+    <row r="3" spans="1:9">
       <c r="B3" s="30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="14" thickBot="1">
       <c r="B4" s="29"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="B5" s="24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="B6" s="25"/>
     </row>
-    <row r="7" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="14" thickBot="1">
       <c r="B7" s="26"/>
     </row>
-    <row r="8" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="14" thickBot="1">
       <c r="B8" s="23"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="B9" s="27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="14" thickBot="1">
       <c r="B10" s="28"/>
     </row>
   </sheetData>
@@ -3034,19 +3392,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.75" style="7"/>
-    <col min="2" max="2" width="24.625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="49.375" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="10.75" style="7"/>
+    <col min="1" max="1" width="10.7109375" style="7"/>
+    <col min="2" max="2" width="24.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="10.7109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="15">
       <c r="A1" s="53" t="s">
         <v>30</v>
       </c>
@@ -3057,229 +3415,234 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30" customHeight="1">
       <c r="A2" s="48" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" customHeight="1">
       <c r="A3" s="48" t="s">
         <v>43</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" customHeight="1">
       <c r="A4" s="48" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" ht="30" customHeight="1">
       <c r="A5" s="48" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" ht="30" customHeight="1">
       <c r="A6" s="48" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="30" customHeight="1">
       <c r="A7" s="48" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C7" s="57" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" customHeight="1">
       <c r="A8" s="48" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" customHeight="1">
       <c r="A9" s="48" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" customHeight="1">
       <c r="A10" s="48" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" ht="30" customHeight="1">
       <c r="A11" s="48" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:3" ht="30" customHeight="1">
       <c r="A12" s="48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B12" s="31" t="s">
         <v>104</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="49" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="30">
+      <c r="A13" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="31" thickBot="1">
+      <c r="A14" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3">
       <c r="C17" s="7"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:3">
       <c r="C18" s="7"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:3">
       <c r="C19" s="7"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:3">
       <c r="C20" s="7"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:3">
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:3">
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:3">
       <c r="C23" s="7"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:3">
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:3">
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:3">
       <c r="C26" s="7"/>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:3">
       <c r="C27" s="7"/>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:3">
       <c r="C28" s="7"/>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:3">
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:3">
       <c r="C30" s="7"/>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:3">
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:3">
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:3">
       <c r="C33" s="7"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:3">
       <c r="C34" s="7"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:3">
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:3">
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:3">
       <c r="C37" s="7"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:3">
       <c r="C38" s="7"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:3">
       <c r="C39" s="7"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:3">
       <c r="C40" s="7"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:3">
       <c r="C41" s="7"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:3">
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:3">
       <c r="C43" s="7"/>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:3">
       <c r="C44" s="7"/>
     </row>
   </sheetData>

</xml_diff>